<commit_message>
Update localhost start config
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/StartConfig/Localhost/StartSceneConfig@s.xlsx
+++ b/Unity/Assets/Config/Excel/StartConfig/Localhost/StartSceneConfig@s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16507" windowHeight="9517" activeTab="1"/>
+    <workbookView windowWidth="21000" windowHeight="13550"/>
   </bookViews>
   <sheets>
     <sheet name="StartSceneConfig" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -56,31 +56,28 @@
     <t>string</t>
   </si>
   <si>
+    <t>NetInner</t>
+  </si>
+  <si>
+    <t>MicroDustRealm</t>
+  </si>
+  <si>
     <t>Realm</t>
   </si>
   <si>
+    <t>MicroDustGate</t>
+  </si>
+  <si>
     <t>Gate</t>
   </si>
   <si>
-    <t>Gate1</t>
-  </si>
-  <si>
-    <t>Gate2</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Match</t>
-  </si>
-  <si>
     <t>Map</t>
   </si>
   <si>
-    <t>Map1</t>
-  </si>
-  <si>
-    <t>Map2</t>
+    <t>Game</t>
   </si>
   <si>
     <t>RouterManager</t>
@@ -106,16 +103,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -136,7 +133,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -144,14 +141,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -159,7 +156,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -167,7 +164,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -175,7 +172,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -183,7 +180,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -191,14 +188,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -206,7 +203,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -214,7 +211,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -222,14 +219,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -237,42 +234,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -586,19 +583,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -748,55 +745,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1094,23 +1091,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:H12"/>
+  <dimension ref="C3:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.35" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="21.1238938053097" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7522123893805" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.6283185840708" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.3716814159292" style="3" customWidth="1"/>
-    <col min="7" max="8" width="13.1238938053097" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.1272727272727" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7545454545455" style="2" customWidth="1"/>
+    <col min="3" max="5" width="12.6272727272727" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.3727272727273" style="3" customWidth="1"/>
+    <col min="7" max="8" width="13.1272727272727" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
+    <row r="3" ht="13.5" spans="3:8">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:8">
+    <row r="4" ht="13.5" spans="3:8">
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" ht="13.5" spans="3:8">
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1187,10 +1184,10 @@
         <v>13</v>
       </c>
       <c r="H6" s="5">
-        <v>30002</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8">
+        <v>30001</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="3:8">
       <c r="C7" s="5">
         <v>2</v>
       </c>
@@ -1200,14 +1197,14 @@
       <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="5">
-        <v>30003</v>
+        <v>30002</v>
       </c>
     </row>
     <row r="8" spans="3:8">
@@ -1221,18 +1218,18 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="5">
-        <v>30004</v>
+        <v>30003</v>
       </c>
     </row>
     <row r="9" spans="3:8">
       <c r="C9" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
@@ -1241,16 +1238,16 @@
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="3:8">
       <c r="C10" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
@@ -1259,48 +1256,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="3:8">
-      <c r="C11" s="5">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="3:8">
-      <c r="C12" s="5">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1314,21 +1281,21 @@
   <sheetPr/>
   <dimension ref="C3:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.35" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="21.1238938053097" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7522123893805" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.6283185840708" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.3716814159292" style="3" customWidth="1"/>
-    <col min="7" max="8" width="13.1238938053097" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.1272727272727" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7545454545455" style="2" customWidth="1"/>
+    <col min="3" max="5" width="12.6272727272727" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.3727272727273" style="3" customWidth="1"/>
+    <col min="7" max="8" width="13.1272727272727" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
+    <row r="3" ht="13.5" spans="3:8">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1348,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:8">
+    <row r="4" ht="13.5" spans="3:8">
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" ht="13.5" spans="3:8">
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1399,10 +1366,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5">
         <v>30300</v>
@@ -1419,10 +1386,10 @@
         <v>3</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H7" s="5">
         <v>30301</v>
@@ -1439,10 +1406,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="5">
         <v>30302</v>
@@ -1459,10 +1426,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="5">
         <v>30303</v>
@@ -1479,10 +1446,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="5">
         <v>30304</v>

</xml_diff>